<commit_message>
Update Plano de organização do trabalho.xlsx
</commit_message>
<xml_diff>
--- a/Plano de organização do trabalho.xlsx
+++ b/Plano de organização do trabalho.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Afonso Silva\GitHub\PACDF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A03364DD-0554-4DEE-B548-597B8043A6E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A5C4C89-C66C-4041-80FF-A6F86913368B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{27699B03-0E23-4BAD-AA71-0F7310ECF60C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Actividade 1: Determinar os objectivos do negócio</t>
   </si>
@@ -84,6 +84,9 @@
   </si>
   <si>
     <t>2- Avaliação inicial de ferramentas e técnicas:</t>
+  </si>
+  <si>
+    <t>Semanas com o progresso de cada passo da atividade</t>
   </si>
 </sst>
 </file>
@@ -435,45 +438,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEF61A1E-A1F1-4701-B96E-D91EEAA5CA1A}">
-  <dimension ref="A1:A37"/>
+  <dimension ref="A1:S37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+      <selection activeCell="O8" sqref="O8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="K1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K4">
+        <v>1</v>
+      </c>
+      <c r="L4">
+        <v>2</v>
+      </c>
+      <c r="M4">
+        <v>3</v>
+      </c>
+      <c r="N4">
+        <v>4</v>
+      </c>
+      <c r="O4">
+        <v>5</v>
+      </c>
+      <c r="P4">
+        <v>6</v>
+      </c>
+      <c r="Q4">
+        <v>7</v>
+      </c>
+      <c r="R4">
+        <v>8</v>
+      </c>
+      <c r="S4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>6</v>
       </c>

</xml_diff>